<commit_message>
Updated the DevTesting_Diversions.xlsx spreadsheet due to the renaming of water users in the model file. This needs to be updated for the dev testing tool to work correctly
</commit_message>
<xml_diff>
--- a/Input Data/DevTesting/DevTesting_Diversions.xlsx
+++ b/Input Data/DevTesting/DevTesting_Diversions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabaker\Projects\Models\MTOM\MTOM_Dir\Input Data\DevTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\crmms\Input Data\DevTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49B7F58-2E36-45CA-AD51-388D02852068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91671397-5E34-44E0-BA30-D449F13F17D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52608" yWindow="12960" windowWidth="28020" windowHeight="15780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UB_diversions" sheetId="1" r:id="rId1"/>
@@ -191,9 +191,6 @@
     <t>California_CU_Schedules.Needles</t>
   </si>
   <si>
-    <t>California_CU_Schedules.OtherLCWSP</t>
-  </si>
-  <si>
     <t>California_CU_Schedules.PaloVerde</t>
   </si>
   <si>
@@ -318,6 +315,9 @@
   </si>
   <si>
     <t>ICS Credits.BiNationalICS_AZ</t>
+  </si>
+  <si>
+    <t>California_CU_Schedules.CaPumpersDvsToPkr</t>
   </si>
 </sst>
 </file>
@@ -665,13 +665,13 @@
       <selection pane="bottomRight" activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -685,7 +685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>43466</v>
       </c>
@@ -699,7 +699,7 @@
         <v>528.29413368594999</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>43497</v>
       </c>
@@ -713,7 +713,7 @@
         <v>518.42084786776798</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>43525</v>
       </c>
@@ -727,7 +727,7 @@
         <v>429.63405223140398</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>43556</v>
       </c>
@@ -741,7 +741,7 @@
         <v>26165.501714380101</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>43586</v>
       </c>
@@ -755,7 +755,7 @@
         <v>47273.4090902479</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>43617</v>
       </c>
@@ -769,7 +769,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>43647</v>
       </c>
@@ -783,7 +783,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>43678</v>
       </c>
@@ -797,7 +797,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>43709</v>
       </c>
@@ -811,7 +811,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>43739</v>
       </c>
@@ -825,7 +825,7 @@
         <v>29999.999999993001</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>43770</v>
       </c>
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>43800</v>
       </c>
@@ -853,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>43831</v>
       </c>
@@ -867,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>43862</v>
       </c>
@@ -881,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>43891</v>
       </c>
@@ -895,7 +895,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>43922</v>
       </c>
@@ -909,7 +909,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>43952</v>
       </c>
@@ -923,7 +923,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>43983</v>
       </c>
@@ -937,7 +937,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>44013</v>
       </c>
@@ -951,7 +951,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>44044</v>
       </c>
@@ -965,7 +965,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>44075</v>
       </c>
@@ -979,7 +979,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>44105</v>
       </c>
@@ -993,7 +993,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>44136</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>44166</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>44197</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>44228</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>44256</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>44287</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>44317</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>44348</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>44378</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>44409</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>44440</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>44470</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>44501</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>44531</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>44562</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>44593</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>44621</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>44652</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>44682</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>44713</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>44743</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44774</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>44805</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>44835</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>44866</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>44896</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>44927</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>44958</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>44986</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>45017</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>45047</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>45078</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>45108</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>45139</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>45170</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>45200</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>45231</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>45261</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>45292</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>45323</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>45352</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>45383</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>45413</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>45444</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>45474</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>45505</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>45536</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>45566</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>45597</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>45627</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>45658</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>45689</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>45717</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>45748</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>45778</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>45809</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>45839</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>45870</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>45901</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>45931</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>45962</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>45992</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>46023</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>46054</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>46082</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>46113</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>46143</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>46174</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>46204</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>46235</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>46266</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>46296</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>46327</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>46357</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>46388</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>46419</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>46447</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>46478</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>46508</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>46539</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>46569</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>46600</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>46631</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>46661</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>46692</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>46722</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>46753</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>46784</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>46813</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>46844</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>46874</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>46905</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>46935</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>46966</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>46997</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <v>47027</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>47058</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
         <v>47088</v>
       </c>
@@ -2375,19 +2375,19 @@
   <dimension ref="A1:BW123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B107" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AU2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E128" sqref="E128"/>
+      <selection pane="bottomRight" activeCell="BF2" sqref="BF2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="75" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="75" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2512,10 +2512,10 @@
         <v>44</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>46</v>
@@ -2527,16 +2527,16 @@
         <v>49</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AW1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AX1" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="AY1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AZ1" s="1" t="s">
         <v>52</v>
@@ -2557,61 +2557,61 @@
         <v>45</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="BG1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BO1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BR1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BI1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BK1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BU1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BP1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BW1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BU1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>77</v>
-      </c>
     </row>
-    <row r="2" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>43405</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>43435</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43466</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>43497</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>43525</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>43556</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>43586</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43617</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43647</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43678</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="12" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43709</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43739</v>
       </c>
@@ -5335,7 +5335,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="14" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43770</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43800</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43831</v>
       </c>
@@ -6016,7 +6016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>43862</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>43891</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>43922</v>
       </c>
@@ -6697,7 +6697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>43952</v>
       </c>
@@ -6924,7 +6924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>43983</v>
       </c>
@@ -7151,7 +7151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>44013</v>
       </c>
@@ -7378,7 +7378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>44044</v>
       </c>
@@ -7605,7 +7605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>44075</v>
       </c>
@@ -7832,7 +7832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>44105</v>
       </c>
@@ -8059,7 +8059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>44136</v>
       </c>
@@ -8286,7 +8286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>44166</v>
       </c>
@@ -8513,7 +8513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>44197</v>
       </c>
@@ -8740,7 +8740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>44228</v>
       </c>
@@ -8967,7 +8967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>44256</v>
       </c>
@@ -9194,7 +9194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>44287</v>
       </c>
@@ -9421,7 +9421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>44317</v>
       </c>
@@ -9648,7 +9648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>44348</v>
       </c>
@@ -9875,7 +9875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>44378</v>
       </c>
@@ -10102,7 +10102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>44409</v>
       </c>
@@ -10329,7 +10329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>44440</v>
       </c>
@@ -10556,7 +10556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>44470</v>
       </c>
@@ -10783,7 +10783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>44501</v>
       </c>
@@ -11010,7 +11010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>44531</v>
       </c>
@@ -11237,7 +11237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>44562</v>
       </c>
@@ -11464,7 +11464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>44593</v>
       </c>
@@ -11691,7 +11691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>44621</v>
       </c>
@@ -11918,7 +11918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>44652</v>
       </c>
@@ -12145,7 +12145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>44682</v>
       </c>
@@ -12372,7 +12372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44713</v>
       </c>
@@ -12599,7 +12599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>44743</v>
       </c>
@@ -12826,7 +12826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>44774</v>
       </c>
@@ -13053,7 +13053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>44805</v>
       </c>
@@ -13280,7 +13280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>44835</v>
       </c>
@@ -13507,7 +13507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>44866</v>
       </c>
@@ -13734,7 +13734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>44896</v>
       </c>
@@ -13961,7 +13961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>44927</v>
       </c>
@@ -14188,7 +14188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>44958</v>
       </c>
@@ -14415,7 +14415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>44986</v>
       </c>
@@ -14642,7 +14642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>45017</v>
       </c>
@@ -14869,7 +14869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>45047</v>
       </c>
@@ -15096,7 +15096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>45078</v>
       </c>
@@ -15323,7 +15323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>45108</v>
       </c>
@@ -15550,7 +15550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>45139</v>
       </c>
@@ -15777,7 +15777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>45170</v>
       </c>
@@ -16004,7 +16004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>45200</v>
       </c>
@@ -16231,7 +16231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>45231</v>
       </c>
@@ -16458,7 +16458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>45261</v>
       </c>
@@ -16685,7 +16685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>45292</v>
       </c>
@@ -16912,7 +16912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>45323</v>
       </c>
@@ -17139,7 +17139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>45352</v>
       </c>
@@ -17366,7 +17366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>45383</v>
       </c>
@@ -17593,7 +17593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>45413</v>
       </c>
@@ -17820,7 +17820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>45444</v>
       </c>
@@ -18047,7 +18047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>45474</v>
       </c>
@@ -18274,7 +18274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>45505</v>
       </c>
@@ -18501,7 +18501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>45536</v>
       </c>
@@ -18728,7 +18728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>45566</v>
       </c>
@@ -18955,7 +18955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>45597</v>
       </c>
@@ -19182,7 +19182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>45627</v>
       </c>
@@ -19409,7 +19409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>45658</v>
       </c>
@@ -19636,7 +19636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>45689</v>
       </c>
@@ -19863,7 +19863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
         <v>45717</v>
       </c>
@@ -20090,7 +20090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
         <v>45748</v>
       </c>
@@ -20317,7 +20317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
         <v>45778</v>
       </c>
@@ -20544,7 +20544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>45809</v>
       </c>
@@ -20771,7 +20771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>45839</v>
       </c>
@@ -20998,7 +20998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
         <v>45870</v>
       </c>
@@ -21225,7 +21225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
         <v>45901</v>
       </c>
@@ -21452,7 +21452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
         <v>45931</v>
       </c>
@@ -21679,7 +21679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
         <v>45962</v>
       </c>
@@ -21906,7 +21906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
         <v>45992</v>
       </c>
@@ -22133,7 +22133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
         <v>46023</v>
       </c>
@@ -22360,7 +22360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
         <v>46054</v>
       </c>
@@ -22587,7 +22587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>46082</v>
       </c>
@@ -22814,7 +22814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
         <v>46113</v>
       </c>
@@ -23041,7 +23041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
         <v>46143</v>
       </c>
@@ -23268,7 +23268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
         <v>46174</v>
       </c>
@@ -23495,7 +23495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
         <v>46204</v>
       </c>
@@ -23722,7 +23722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
         <v>46235</v>
       </c>
@@ -23949,7 +23949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
         <v>46266</v>
       </c>
@@ -24176,7 +24176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
         <v>46296</v>
       </c>
@@ -24403,7 +24403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
         <v>46327</v>
       </c>
@@ -24630,7 +24630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
         <v>46357</v>
       </c>
@@ -24857,7 +24857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
         <v>46388</v>
       </c>
@@ -25084,7 +25084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
         <v>46419</v>
       </c>
@@ -25311,7 +25311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
         <v>46447</v>
       </c>
@@ -25538,7 +25538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
         <v>46478</v>
       </c>
@@ -25765,7 +25765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
         <v>46508</v>
       </c>
@@ -25992,7 +25992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
         <v>46539</v>
       </c>
@@ -26219,7 +26219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
         <v>46569</v>
       </c>
@@ -26446,7 +26446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A107" s="4">
         <v>46600</v>
       </c>
@@ -26673,7 +26673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
         <v>46631</v>
       </c>
@@ -26900,7 +26900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A109" s="4">
         <v>46661</v>
       </c>
@@ -27127,7 +27127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A110" s="4">
         <v>46692</v>
       </c>
@@ -27354,7 +27354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A111" s="4">
         <v>46722</v>
       </c>
@@ -27581,7 +27581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A112" s="4">
         <v>46753</v>
       </c>
@@ -27808,7 +27808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A113" s="4">
         <v>46784</v>
       </c>
@@ -28035,7 +28035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A114" s="4">
         <v>46813</v>
       </c>
@@ -28262,7 +28262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A115" s="4">
         <v>46844</v>
       </c>
@@ -28489,7 +28489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A116" s="4">
         <v>46874</v>
       </c>
@@ -28716,7 +28716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A117" s="4">
         <v>46905</v>
       </c>
@@ -28943,7 +28943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A118" s="4">
         <v>46935</v>
       </c>
@@ -29170,7 +29170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A119" s="4">
         <v>46966</v>
       </c>
@@ -29397,7 +29397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A120" s="4">
         <v>46997</v>
       </c>
@@ -29624,7 +29624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A121" s="4">
         <v>47027</v>
       </c>
@@ -29851,10 +29851,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A122" s="4"/>
     </row>
-    <row r="123" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A123" s="4"/>
     </row>
   </sheetData>
@@ -29870,77 +29870,77 @@
       <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="20" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" customWidth="1"/>
+    <col min="11" max="20" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>40179</v>
       </c>
@@ -30002,7 +30002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>40544</v>
       </c>
@@ -30064,7 +30064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>40909</v>
       </c>
@@ -30126,7 +30126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>41275</v>
       </c>
@@ -30188,7 +30188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>41640</v>
       </c>
@@ -30250,7 +30250,7 @@
         <v>21375</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>42005</v>
       </c>
@@ -30312,7 +30312,7 @@
         <v>23890</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>42370</v>
       </c>
@@ -30374,7 +30374,7 @@
         <v>21171</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>42736</v>
       </c>
@@ -30436,7 +30436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>43101</v>
       </c>
@@ -30498,7 +30498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>43466</v>
       </c>
@@ -30560,7 +30560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>43831</v>
       </c>
@@ -30622,7 +30622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44197</v>
       </c>
@@ -30684,7 +30684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>44562</v>
       </c>
@@ -30746,7 +30746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>44927</v>
       </c>
@@ -30808,7 +30808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45292</v>
       </c>
@@ -30870,7 +30870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>45658</v>
       </c>
@@ -30932,7 +30932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>46023</v>
       </c>

</xml_diff>

<commit_message>
update Ranch5 to FYIR_Ranches in input diversion spreadsheet
</commit_message>
<xml_diff>
--- a/Input Data/DevTesting/DevTesting_Diversions.xlsx
+++ b/Input Data/DevTesting/DevTesting_Diversions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20383"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\crmms\Input Data\DevTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saba3704\Documents\crmms\Input Data\DevTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91671397-5E34-44E0-BA30-D449F13F17D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04307428-DF21-40D6-9970-CD2DE948420F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52608" yWindow="12960" windowWidth="28020" windowHeight="15780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52605" yWindow="12960" windowWidth="28020" windowHeight="15780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UB_diversions" sheetId="1" r:id="rId1"/>
@@ -194,9 +194,6 @@
     <t>California_CU_Schedules.PaloVerde</t>
   </si>
   <si>
-    <t>California_CU_Schedules.Ranch5</t>
-  </si>
-  <si>
     <t>California_CU_Schedules.SaltonSea</t>
   </si>
   <si>
@@ -318,6 +315,9 @@
   </si>
   <si>
     <t>California_CU_Schedules.CaPumpersDvsToPkr</t>
+  </si>
+  <si>
+    <t>California_CU_Schedules.FYIR_Ranches</t>
   </si>
 </sst>
 </file>
@@ -665,13 +665,13 @@
       <selection pane="bottomRight" activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -685,7 +685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43466</v>
       </c>
@@ -699,7 +699,7 @@
         <v>528.29413368594999</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43497</v>
       </c>
@@ -713,7 +713,7 @@
         <v>518.42084786776798</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43525</v>
       </c>
@@ -727,7 +727,7 @@
         <v>429.63405223140398</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43556</v>
       </c>
@@ -741,7 +741,7 @@
         <v>26165.501714380101</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43586</v>
       </c>
@@ -755,7 +755,7 @@
         <v>47273.4090902479</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43617</v>
       </c>
@@ -769,7 +769,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43647</v>
       </c>
@@ -783,7 +783,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>43678</v>
       </c>
@@ -797,7 +797,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43709</v>
       </c>
@@ -811,7 +811,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43739</v>
       </c>
@@ -825,7 +825,7 @@
         <v>29999.999999993001</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43770</v>
       </c>
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43800</v>
       </c>
@@ -853,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43831</v>
       </c>
@@ -867,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43862</v>
       </c>
@@ -881,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43891</v>
       </c>
@@ -895,7 +895,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>43922</v>
       </c>
@@ -909,7 +909,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43952</v>
       </c>
@@ -923,7 +923,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43983</v>
       </c>
@@ -937,7 +937,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44013</v>
       </c>
@@ -951,7 +951,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44044</v>
       </c>
@@ -965,7 +965,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44075</v>
       </c>
@@ -979,7 +979,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44105</v>
       </c>
@@ -993,7 +993,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44136</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44166</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44197</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44228</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44256</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44287</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44317</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44348</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44378</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44409</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44440</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44470</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44501</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44531</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44562</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44593</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44621</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>44652</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>44682</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>44713</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>44743</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44774</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44805</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44835</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>44866</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>44896</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>44927</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>44958</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>44986</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>45017</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>45047</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>45078</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>45108</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>45139</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>45170</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>45200</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>45231</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>45261</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>45292</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>45323</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>45352</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>45383</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>45413</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>45444</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>45474</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>45505</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>45536</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>45566</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>45597</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>45627</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>45658</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>45689</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>45717</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>45748</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>45778</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>45809</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>45839</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>45870</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>45901</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>45931</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>45962</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>45992</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>46023</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>46054</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>46082</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>46113</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>46143</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>46174</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>46204</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>46235</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>46266</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>46296</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>46327</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>46357</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>46388</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>46419</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>46447</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>46478</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>46508</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>46539</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>46569</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>46600</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>46631</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>46661</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>46692</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>46722</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>46753</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>46784</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>46813</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>4999.9999999915899</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>46844</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>41999.999999957901</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>46874</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>61999.999999999702</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>46905</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>61000.000000083899</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>46935</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>46966</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>65000.000000020897</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>46997</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>47027</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>47058</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>47088</v>
       </c>
@@ -2375,19 +2375,19 @@
   <dimension ref="A1:BW123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AU2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BF2" sqref="BF2"/>
+      <selection pane="bottomRight" activeCell="AQ2" sqref="AQ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="75" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="75" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:75" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2512,10 +2512,10 @@
         <v>44</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>46</v>
@@ -2530,13 +2530,13 @@
         <v>54</v>
       </c>
       <c r="AW1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AX1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AX1" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="AY1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AZ1" s="1" t="s">
         <v>52</v>
@@ -2557,61 +2557,61 @@
         <v>45</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BG1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BO1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BR1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BI1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BK1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BU1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BP1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BU1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>76</v>
-      </c>
     </row>
-    <row r="2" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>43405</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>43435</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>43466</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>43497</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>43525</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>43556</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:75" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>43586</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>43617</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>43647</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>43678</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="12" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>43709</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>43739</v>
       </c>
@@ -5335,7 +5335,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="14" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>43770</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>43800</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>43831</v>
       </c>
@@ -6016,7 +6016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>43862</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>43891</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>43922</v>
       </c>
@@ -6697,7 +6697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>43952</v>
       </c>
@@ -6924,7 +6924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>43983</v>
       </c>
@@ -7151,7 +7151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>44013</v>
       </c>
@@ -7378,7 +7378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>44044</v>
       </c>
@@ -7605,7 +7605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>44075</v>
       </c>
@@ -7832,7 +7832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>44105</v>
       </c>
@@ -8059,7 +8059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>44136</v>
       </c>
@@ -8286,7 +8286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>44166</v>
       </c>
@@ -8513,7 +8513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>44197</v>
       </c>
@@ -8740,7 +8740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>44228</v>
       </c>
@@ -8967,7 +8967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>44256</v>
       </c>
@@ -9194,7 +9194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>44287</v>
       </c>
@@ -9421,7 +9421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>44317</v>
       </c>
@@ -9648,7 +9648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>44348</v>
       </c>
@@ -9875,7 +9875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>44378</v>
       </c>
@@ -10102,7 +10102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>44409</v>
       </c>
@@ -10329,7 +10329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>44440</v>
       </c>
@@ -10556,7 +10556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>44470</v>
       </c>
@@ -10783,7 +10783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>44501</v>
       </c>
@@ -11010,7 +11010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>44531</v>
       </c>
@@ -11237,7 +11237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>44562</v>
       </c>
@@ -11464,7 +11464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>44593</v>
       </c>
@@ -11691,7 +11691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>44621</v>
       </c>
@@ -11918,7 +11918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>44652</v>
       </c>
@@ -12145,7 +12145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>44682</v>
       </c>
@@ -12372,7 +12372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>44713</v>
       </c>
@@ -12599,7 +12599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>44743</v>
       </c>
@@ -12826,7 +12826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>44774</v>
       </c>
@@ -13053,7 +13053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>44805</v>
       </c>
@@ -13280,7 +13280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>44835</v>
       </c>
@@ -13507,7 +13507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>44866</v>
       </c>
@@ -13734,7 +13734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>44896</v>
       </c>
@@ -13961,7 +13961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>44927</v>
       </c>
@@ -14188,7 +14188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>44958</v>
       </c>
@@ -14415,7 +14415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>44986</v>
       </c>
@@ -14642,7 +14642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>45017</v>
       </c>
@@ -14869,7 +14869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>45047</v>
       </c>
@@ -15096,7 +15096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>45078</v>
       </c>
@@ -15323,7 +15323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>45108</v>
       </c>
@@ -15550,7 +15550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>45139</v>
       </c>
@@ -15777,7 +15777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>45170</v>
       </c>
@@ -16004,7 +16004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>45200</v>
       </c>
@@ -16231,7 +16231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>45231</v>
       </c>
@@ -16458,7 +16458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>45261</v>
       </c>
@@ -16685,7 +16685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>45292</v>
       </c>
@@ -16912,7 +16912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>45323</v>
       </c>
@@ -17139,7 +17139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>45352</v>
       </c>
@@ -17366,7 +17366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>45383</v>
       </c>
@@ -17593,7 +17593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>45413</v>
       </c>
@@ -17820,7 +17820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>45444</v>
       </c>
@@ -18047,7 +18047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>45474</v>
       </c>
@@ -18274,7 +18274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>45505</v>
       </c>
@@ -18501,7 +18501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>45536</v>
       </c>
@@ -18728,7 +18728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>45566</v>
       </c>
@@ -18955,7 +18955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>45597</v>
       </c>
@@ -19182,7 +19182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>45627</v>
       </c>
@@ -19409,7 +19409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>45658</v>
       </c>
@@ -19636,7 +19636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>45689</v>
       </c>
@@ -19863,7 +19863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>45717</v>
       </c>
@@ -20090,7 +20090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>45748</v>
       </c>
@@ -20317,7 +20317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>45778</v>
       </c>
@@ -20544,7 +20544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>45809</v>
       </c>
@@ -20771,7 +20771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>45839</v>
       </c>
@@ -20998,7 +20998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>45870</v>
       </c>
@@ -21225,7 +21225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>45901</v>
       </c>
@@ -21452,7 +21452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>45931</v>
       </c>
@@ -21679,7 +21679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>45962</v>
       </c>
@@ -21906,7 +21906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>45992</v>
       </c>
@@ -22133,7 +22133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>46023</v>
       </c>
@@ -22360,7 +22360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>46054</v>
       </c>
@@ -22587,7 +22587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>46082</v>
       </c>
@@ -22814,7 +22814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>46113</v>
       </c>
@@ -23041,7 +23041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>46143</v>
       </c>
@@ -23268,7 +23268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>46174</v>
       </c>
@@ -23495,7 +23495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>46204</v>
       </c>
@@ -23722,7 +23722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>46235</v>
       </c>
@@ -23949,7 +23949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>46266</v>
       </c>
@@ -24176,7 +24176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>46296</v>
       </c>
@@ -24403,7 +24403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>46327</v>
       </c>
@@ -24630,7 +24630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>46357</v>
       </c>
@@ -24857,7 +24857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>46388</v>
       </c>
@@ -25084,7 +25084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>46419</v>
       </c>
@@ -25311,7 +25311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>46447</v>
       </c>
@@ -25538,7 +25538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>46478</v>
       </c>
@@ -25765,7 +25765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>46508</v>
       </c>
@@ -25992,7 +25992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>46539</v>
       </c>
@@ -26219,7 +26219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>46569</v>
       </c>
@@ -26446,7 +26446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>46600</v>
       </c>
@@ -26673,7 +26673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>46631</v>
       </c>
@@ -26900,7 +26900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>46661</v>
       </c>
@@ -27127,7 +27127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>46692</v>
       </c>
@@ -27354,7 +27354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>46722</v>
       </c>
@@ -27581,7 +27581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>46753</v>
       </c>
@@ -27808,7 +27808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>46784</v>
       </c>
@@ -28035,7 +28035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>46813</v>
       </c>
@@ -28262,7 +28262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>46844</v>
       </c>
@@ -28489,7 +28489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>46874</v>
       </c>
@@ -28716,7 +28716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>46905</v>
       </c>
@@ -28943,7 +28943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>46935</v>
       </c>
@@ -29170,7 +29170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>46966</v>
       </c>
@@ -29397,7 +29397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>46997</v>
       </c>
@@ -29624,7 +29624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>47027</v>
       </c>
@@ -29851,10 +29851,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
     </row>
-    <row r="123" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
     </row>
   </sheetData>
@@ -29870,77 +29870,77 @@
       <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="18.44140625" customWidth="1"/>
-    <col min="11" max="20" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="20" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>40179</v>
       </c>
@@ -30002,7 +30002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>40544</v>
       </c>
@@ -30064,7 +30064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>40909</v>
       </c>
@@ -30126,7 +30126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>41275</v>
       </c>
@@ -30188,7 +30188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>41640</v>
       </c>
@@ -30250,7 +30250,7 @@
         <v>21375</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>42005</v>
       </c>
@@ -30312,7 +30312,7 @@
         <v>23890</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>42370</v>
       </c>
@@ -30374,7 +30374,7 @@
         <v>21171</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>42736</v>
       </c>
@@ -30436,7 +30436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43101</v>
       </c>
@@ -30498,7 +30498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43466</v>
       </c>
@@ -30560,7 +30560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43831</v>
       </c>
@@ -30622,7 +30622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44197</v>
       </c>
@@ -30684,7 +30684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44562</v>
       </c>
@@ -30746,7 +30746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44927</v>
       </c>
@@ -30808,7 +30808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45292</v>
       </c>
@@ -30870,7 +30870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45658</v>
       </c>
@@ -30932,7 +30932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>46023</v>
       </c>

</xml_diff>